<commit_message>
Updated Lia's kidney AKI biomarker data
</commit_message>
<xml_diff>
--- a/docs/kidney_biomarkers/AKI_biomarkers-Lia.xlsx
+++ b/docs/kidney_biomarkers/AKI_biomarkers-Lia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yongqunh\GitHub\KTAO\docs\kidney_biomarkers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23AE331-129B-431F-9FB6-B2B8A83F669A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3244F17-F675-4AF4-ABEC-7416982C9AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9085" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9087" uniqueCount="595">
   <si>
     <t>Synonym Gene Symbol</t>
   </si>
@@ -2083,6 +2083,9 @@
   <si>
     <t>PR_000018880</t>
   </si>
+  <si>
+    <t>AAG4</t>
+  </si>
 </sst>
 </file>
 
@@ -2702,8 +2705,8 @@
   </sheetPr>
   <dimension ref="A1:AJ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4481,18 +4484,24 @@
       <c r="AJ24" s="4"/>
     </row>
     <row r="25" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C25" s="5"/>
+      <c r="A25" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>594</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1191</v>
+      </c>
       <c r="D25" s="82" t="s">
         <v>592</v>
       </c>
       <c r="E25" s="56" t="s">
         <v>591</v>
       </c>
-      <c r="F25" s="5"/>
+      <c r="F25" s="20" t="s">
+        <v>220</v>
+      </c>
       <c r="G25" s="5" t="s">
         <v>25</v>
       </c>
@@ -41887,6 +41896,7 @@
     <hyperlink ref="Q47" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId78"/>
 </worksheet>
 </file>
 

</xml_diff>